<commit_message>
NPV Calculation for traditional approach complete
</commit_message>
<xml_diff>
--- a/Sample.xlsx
+++ b/Sample.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://zhaw-my.sharepoint.com/personal/bieriol1_students_zhaw_ch/Documents/Master AV/Semester 1/VT1/Python files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://zhaw-my.sharepoint.com/personal/bieriol1_students_zhaw_ch/Documents/Master AV/Semester 1/VT1/VT1-Python-Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="10" documentId="11_AD4DB114E441178AC67DF4E7D654E4C4693EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC4FF9DD-651A-4ED4-8769-498C7D136C68}"/>
@@ -103,8 +103,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Prozent" xfId="1" builtinId="5"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -388,7 +388,7 @@
       <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="2" max="2" width="9.6796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.86328125" bestFit="1" customWidth="1"/>

</xml_diff>